<commit_message>
Implement getting data by id and deleting data
</commit_message>
<xml_diff>
--- a/API/Data/sample-xlsx-file-for-testing.xlsx
+++ b/API/Data/sample-xlsx-file-for-testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Segment</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>Dobalina</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
 </sst>
 </file>
@@ -813,7 +807,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P702"/>
+  <dimension ref="A1:P701"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A689" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D697" sqref="D697"/>
@@ -35887,56 +35881,6 @@
       </c>
       <c r="P701" s="9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="702">
-      <c r="A702" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B702" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C702" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D702" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E702" s="3">
-        <v>0</v>
-      </c>
-      <c r="F702" s="3">
-        <v>0</v>
-      </c>
-      <c r="G702" s="3">
-        <v>0</v>
-      </c>
-      <c r="H702" s="3">
-        <v>0</v>
-      </c>
-      <c r="I702" s="3">
-        <v>0</v>
-      </c>
-      <c r="J702" s="3">
-        <v>0</v>
-      </c>
-      <c r="K702" s="2">
-        <v>0</v>
-      </c>
-      <c r="L702" s="2">
-        <v>0</v>
-      </c>
-      <c r="M702" s="6">
-        <v>44631.78395134259</v>
-      </c>
-      <c r="N702" s="11">
-        <v>0</v>
-      </c>
-      <c r="O702" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P702" s="4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check if row has data when removing it, return true if removed.
</commit_message>
<xml_diff>
--- a/API/Data/sample-xlsx-file-for-testing.xlsx
+++ b/API/Data/sample-xlsx-file-for-testing.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pryq1\source\repos\API\API\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pryq1\source\repos\AJP-RadoslawRadomski\API\API\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19891FDF-B8D5-4294-8B23-2E55E8F7AF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F65BD1DB-2538-4EEF-8E0E-C417012CAE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -809,28 +810,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A689" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D697" sqref="D697"/>
+    <sheetView tabSelected="1" topLeftCell="D698" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M704" sqref="M704"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="16.28515625" customWidth="1" style="2"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1" style="2"/>
-    <col min="3" max="3" bestFit="1" width="14.140625" customWidth="1" style="5"/>
-    <col min="4" max="4" bestFit="1" width="17.42578125" customWidth="1" style="2"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" style="3"/>
-    <col min="6" max="6" bestFit="1" width="14.28515625" customWidth="1" style="3"/>
-    <col min="7" max="7" bestFit="1" width="12.5703125" customWidth="1" style="3"/>
-    <col min="8" max="8" bestFit="1" width="14.28515625" customWidth="1" style="3"/>
-    <col min="9" max="9" bestFit="1" width="12.5703125" customWidth="1" style="3"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1" style="3"/>
-    <col min="11" max="11" bestFit="1" width="11.5703125" customWidth="1" style="2"/>
-    <col min="12" max="12" bestFit="1" width="18.42578125" customWidth="1" style="2"/>
-    <col min="13" max="13" bestFit="1" width="11.5703125" customWidth="1" style="6"/>
-    <col min="14" max="14" bestFit="1" width="17.140625" customWidth="1" style="11"/>
-    <col min="15" max="15" bestFit="1" width="16.5703125" customWidth="1" style="2"/>
-    <col min="16" max="16" bestFit="1" width="7.5703125" customWidth="1" style="4"/>
+    <col min="1" max="1" bestFit="1" width="16.26953125" customWidth="1" style="2"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1" style="2"/>
+    <col min="3" max="3" bestFit="1" width="14.1328125" customWidth="1" style="5"/>
+    <col min="4" max="4" bestFit="1" width="17.40625" customWidth="1" style="2"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1" style="3"/>
+    <col min="6" max="6" bestFit="1" width="14.26953125" customWidth="1" style="3"/>
+    <col min="7" max="7" bestFit="1" width="12.54296875" customWidth="1" style="3"/>
+    <col min="8" max="8" bestFit="1" width="14.26953125" customWidth="1" style="3"/>
+    <col min="9" max="9" bestFit="1" width="12.54296875" customWidth="1" style="3"/>
+    <col min="10" max="10" width="17.7265625" customWidth="1" style="3"/>
+    <col min="11" max="11" bestFit="1" width="11.54296875" customWidth="1" style="2"/>
+    <col min="12" max="12" bestFit="1" width="18.40625" customWidth="1" style="2"/>
+    <col min="13" max="13" bestFit="1" width="11.54296875" customWidth="1" style="6"/>
+    <col min="14" max="14" bestFit="1" width="17.1328125" customWidth="1" style="11"/>
+    <col min="15" max="15" bestFit="1" width="16.54296875" customWidth="1" style="2"/>
+    <col min="16" max="16" bestFit="1" width="7.54296875" customWidth="1" style="4"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Extract date infor from original date to simplify adding new rows.
</commit_message>
<xml_diff>
--- a/API/Data/sample-xlsx-file-for-testing.xlsx
+++ b/API/Data/sample-xlsx-file-for-testing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Segment</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>bomfunk</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -808,7 +814,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P701"/>
+  <dimension ref="A1:P702"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D698" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M704" sqref="M704"/>
@@ -35882,6 +35888,47 @@
       </c>
       <c r="P701" s="9" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B702" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C702" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D702" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E702" s="3">
+        <v>0</v>
+      </c>
+      <c r="F702" s="3">
+        <v>0</v>
+      </c>
+      <c r="G702" s="3">
+        <v>0</v>
+      </c>
+      <c r="H702" s="3">
+        <v>0</v>
+      </c>
+      <c r="I702" s="3">
+        <v>0</v>
+      </c>
+      <c r="J702" s="3">
+        <v>0</v>
+      </c>
+      <c r="K702" s="2">
+        <v>0</v>
+      </c>
+      <c r="L702" s="2">
+        <v>0</v>
+      </c>
+      <c r="M702" s="6">
+        <v>44632.28408965278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use GroupBy in generating reports
</commit_message>
<xml_diff>
--- a/API/Data/sample-xlsx-file-for-testing.xlsx
+++ b/API/Data/sample-xlsx-file-for-testing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Segment</t>
   </si>
@@ -176,12 +176,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>bomfunk</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
 </sst>
 </file>
@@ -814,7 +808,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P702"/>
+  <dimension ref="A1:P701"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D698" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M704" sqref="M704"/>
@@ -35888,47 +35882,6 @@
       </c>
       <c r="P701" s="9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="702">
-      <c r="A702" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B702" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C702" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D702" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E702" s="3">
-        <v>0</v>
-      </c>
-      <c r="F702" s="3">
-        <v>0</v>
-      </c>
-      <c r="G702" s="3">
-        <v>0</v>
-      </c>
-      <c r="H702" s="3">
-        <v>0</v>
-      </c>
-      <c r="I702" s="3">
-        <v>0</v>
-      </c>
-      <c r="J702" s="3">
-        <v>0</v>
-      </c>
-      <c r="K702" s="2">
-        <v>0</v>
-      </c>
-      <c r="L702" s="2">
-        <v>0</v>
-      </c>
-      <c r="M702" s="6">
-        <v>44632.28408965278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>